<commit_message>
Parts list for v2
</commit_message>
<xml_diff>
--- a/Partlist/partlist.xlsx
+++ b/Partlist/partlist.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramon\Documents\GitHub\RobotBjorn\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramon\Documents\GitHub\RobotBjorn\Partlist\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Product Name</t>
   </si>
@@ -47,12 +47,6 @@
     <t>Chassis</t>
   </si>
   <si>
-    <t>Arduino Uno</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arduino Motorshield </t>
-  </si>
-  <si>
     <t>Product URL</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
     <t>Range Sensors</t>
   </si>
   <si>
-    <t>Bluetooth Module</t>
-  </si>
-  <si>
     <t>Adjustable Infrared Sensor Switch</t>
   </si>
   <si>
@@ -87,6 +78,33 @@
   </si>
   <si>
     <t>Horn</t>
+  </si>
+  <si>
+    <t>http://arduino.cc/en/Main/ArduinoMotorShieldR3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arduino Motor Shield R3 </t>
+  </si>
+  <si>
+    <t>Arduino Uno R3</t>
+  </si>
+  <si>
+    <t>Motor Shield</t>
+  </si>
+  <si>
+    <t>Core</t>
+  </si>
+  <si>
+    <t>http://www.arduino.cc/en/Main/arduinoBoardUno</t>
+  </si>
+  <si>
+    <t>http://www.dfrobot.com/index.php?route=product/product&amp;product_id=97</t>
+  </si>
+  <si>
+    <t>Kingbright</t>
+  </si>
+  <si>
+    <t>Kingbright Ultra Red</t>
   </si>
 </sst>
 </file>
@@ -161,8 +179,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:F10" totalsRowShown="0">
-  <autoFilter ref="A1:F10"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="A1:F9" totalsRowShown="0">
+  <autoFilter ref="A1:F9"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Product Name"/>
     <tableColumn id="2" name="Product Number"/>
@@ -438,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,7 +489,7 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -479,7 +497,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -490,42 +508,75 @@
       <c r="E2">
         <v>1</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>19</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
+      <c r="F4" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.25</v>
       </c>
       <c r="E5">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.25</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>11</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.25</v>
       </c>
       <c r="E7">
         <v>4</v>
@@ -533,48 +584,43 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E8">
         <v>3</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F8" r:id="rId1"/>
+    <hyperlink ref="F4" r:id="rId2"/>
+    <hyperlink ref="F3" r:id="rId3"/>
+    <hyperlink ref="F2" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>